<commit_message>
First good attempt, untested
</commit_message>
<xml_diff>
--- a/utils/examples.xlsx
+++ b/utils/examples.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365tno.sharepoint.com/teams/P060.37572/TeamDocuments/External Audience/Credential Catalogue/Example credentials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\bart\devel\credential-catalogue-ckan\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{911E2177-8877-45F6-99EC-B78D65F4F627}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{753009D6-A41E-4704-9BF9-240800849B7C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526A549B-3794-424A-B5EC-A0F7D0EA3998}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{97384346-CD31-4D68-82C9-54529F88DA6A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -93,48 +93,9 @@
     <t>Esatus</t>
   </si>
   <si>
-    <t>Complete</t>
-  </si>
-  <si>
     <t>As many employees are involved in several projects, either internally or for third parties, i.e. clients, a separate schema reflecting project memberships was required. Typically, a project has a name and an identifier and an employee has a specific role in it.</t>
   </si>
   <si>
-    <t>TxID: Ar1YzNwcM74M2Z4XKUWXMW:2:
-EmploymentSchema:1.0, Seqno: 54019
-employer
-employeeID
-userID
-email
-employmentType
-issuingDate
-expiryDate
-https://esatus.com/files/whitepapers/esatus_SSI_Roll-out.pdf</t>
-  </si>
-  <si>
-    <t>TxID: Ar1YzNwcM74M2Z4XKUWXMW:2:
-DepartmentMemberSchema:1.0, Seqno: 54020
-position
-location
-departmentID
-department
-issuingDate
-expiryDate
-https://esatus.com/files/whitepapers/esatus_SSI_Roll-out.pdf</t>
-  </si>
-  <si>
-    <t>TxID: Ar1YzNwcM74M2Z4XKUWXMW:2:
-ProjectMemberSchema:1.0, Seqno: 54021
-role
-projectID
-project
-issuingDate
-expiryDate
-https://esatus.com/files/whitepapers/esatus_SSI_Roll-out.pdf</t>
-  </si>
-  <si>
-    <t>for internal use</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -150,7 +111,243 @@
     <t>DiplomaCredential</t>
   </si>
   <si>
-    <t>Credential made for EBIS4austria that asserts a student has a diploma. Examples:
+    <t>DataKeeper name credential</t>
+  </si>
+  <si>
+    <t>A name as retrieved from a passport</t>
+  </si>
+  <si>
+    <t>VC, datakeeper</t>
+  </si>
+  <si>
+    <t>Marnix.van.den.Bent@rabobank.nl</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>INDY ledger</t>
+  </si>
+  <si>
+    <t>ggirc-act.ghg-emissions-report</t>
+  </si>
+  <si>
+    <t>0.2.1</t>
+  </si>
+  <si>
+    <t>Farm_Schema</t>
+  </si>
+  <si>
+    <t>COVID-19 Test Result</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>COVID-19 Vaccine</t>
+  </si>
+  <si>
+    <t>112.11</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/RoosBakker/coti</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>documentation</t>
+  </si>
+  <si>
+    <t>supportedProts</t>
+  </si>
+  <si>
+    <t>maturity</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Stores the result of a LAMP quicktest for COVID 19</t>
+  </si>
+  <si>
+    <t>Stores the result of an antigetn quicktest for COVID 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credential made for EBIS4austria that asserts a student has a diploma.
+</t>
+  </si>
+  <si>
+    <t>See example</t>
+  </si>
+  <si>
+    <t>BSN from healthcare</t>
+  </si>
+  <si>
+    <t>https://privacybydesign.foundation/attribute-index/en/pbdf.chipsoft.bsn.html</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>https://privacybydesign.foundation/attribute-index/en/pbdf.bzkpilot.address.html</t>
+  </si>
+  <si>
+    <t>https://privacybydesign.foundation/attribute-index/en/pbdf.bzkpilot.personalData.html</t>
+  </si>
+  <si>
+    <t>IRMA</t>
+  </si>
+  <si>
+    <t>Personal data</t>
+  </si>
+  <si>
+    <t>AGB code</t>
+  </si>
+  <si>
+    <t>https://privacybydesign.foundation/attribute-index/en/pbdf.nuts.agb.html</t>
+  </si>
+  <si>
+    <t>pilot</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>```
+{
+  "@context": [
+    "https://www.w3.org/2018/credentials/v1",
+    "https://www.tno.nl/health/ontology/coti" // TODO: location of schema
+  ],
+  "id": "https://ns.unlock.nl/credentials/example/2",
+  "type": ["VerifiableCredential", "COVID19LAMPTestResultCredential"],
+  "issuer": "did:example:c276e12ec21ebfeb1f712ebc6f1",
+  "issuanceDate": "2020-12-10T19:73:24Z",
+  "credentialSubject": {
+    "id": "did:example:ebfeb1f712ebc6f1c276e12ec21", // did of unlock wallet
+    "passportPhotograph": "iVBORw0KGgoAAAANSUhEUgAAAuAAAACFCAIAAACVGtqeAAAAA3", // string of the image
+    "testResult": {
+      "date": "2020-12-10T00:00:00Z", // datetime on which the test result is specified
+      "result": false,
+      "usedTest": {
+        "testName": "TNOLAMP",
+        "testType": "LAMP based SARS-CoV-2 test",
+        "doneByLab": {
+          "id": "https://tno.nl", // identifier of test laboratory
+          "name": "TNO"
+        }
+      }
+    }
+  },
+  "proof": {
+    "type": "RsaSignature2018",
+    "created": "2017-06-18T21:19:10Z",
+    "proofPurpose": "assertionMethod",
+    "verificationMethod": "https://example.edu/issuers/keys/1",
+    "jws": "eyJhbGciOiJSUzI1NiIsImI2NCI6ZmFsc2UsImNyaXQiOlsiYjY0Il19..TCYt5XsITJX1CxPCT8yAV-TVkIEq_PbChOMqsLfRoPsnsgw5WEuts01mq-pQy7UJiN5mgRxD-WUcX16dUEMGlv50aqzpqh4Qktb3rk-BuQy72IFLOqV0G_zS245-kronKb78cPN25DGlcTwLtjPAYuNzVBAh4vGHSrQyHUdBBPM"
+  }
+}
+```</t>
+  </si>
+  <si>
+    <t>```
+{
+  "+D5@context": [
+    "https://www.w3.org/2018/credentials/v1",
+    "https://www.tno.nl/health/ontology/coti" // TODO: location of schema
+  ],
+  "id": "https://ns.unlock.nl/credentials/example/2",
+  "type": ["VerifiableCredential", "COVID19AntigenTestResultCredential"],
+  "issuer": "did:example:c276e12ec21ebfeb1f712ebc6f1",
+  "issuanceDate": "2020-12-10T19:73:24Z",
+  "credentialSubject": {
+    "id": "did:example:ebfeb1f712ebc6f1c276e12ec21", // did of unlock wallet
+    "passportPhotograph": "iVBORw0KGgoAAAANSUhEUgAAAuAAAACFCAIAAACVGtqeAAAAA3", // string of the image
+    "testResult": {
+      "date": "2020-12-10T00:00:00Z", // datetime on which the test result is specified
+      "result": false,
+      "usedTest": {
+        "testName": "Abbott",
+        "testType": "Antigen based SARS-CoV-2 test",
+        "doneByLab": {
+          "id": "https://ems.eu", // identifier of test laboratory
+          "name": "EMS"
+        }
+      }
+    }
+  },
+  "proof": {
+    "type": "RsaSignature2018",
+    "created": "2017-06-18T21:19:10Z",
+    "proofPurpose": "assertionMethod",
+    "verificationMethod": "https://example.edu/issuers/keys/1",
+    "jws": "eyJhbGciOiJSUzI1NiIsImI2NCI6ZmFsc2UsImNyaXQiOlsiYjY0Il19..TCYt5XsITJX1CxPCT8yAV-TVkIEq_PbChOMqsLfRoPsnsgw5WEuts01mq-pQy7UJiN5mgRxD-WUcX16dUEMGlv50aqzpqh4Qktb3rk-BuQy72IFLOqV0G_zS245-kronKb78cPN25DGlcTwLtjPAYuNzVBAh4vGHSrQyHUdBBPM"
+  }
+}
+```</t>
+  </si>
+  <si>
+    <t>```
+{
+  "@context": [
+    "https://www.w3.org/2018/credentials/v1",
+    "https://www.tno.nl/health/ontology/coti" // TODO: location of schema
+  ],
+  "id": "https://ns.unlock.nl/credentials/example/1",
+  "type": ["VerifiableCredential", "COVID19PCRTestResultCredential"],
+  "issuer": "did:example:c276e12ec21ebfeb1f712ebc6f1",
+  "issuanceDate": "2020-06-06T19:73:24Z",
+  "credentialSubject": {
+    "id": "did:example:ebfeb1f712ebc6f1c276e12ec21", // did of unlock wallet
+    "familyName": "Doe",
+    "givenNames": "John Gerard",
+    "birthDate": "1980-01-01",
+    "testResult": {
+      "date": "2020-06-06T00:00:00Z", // datetime on which the test result is specified
+      "result": false,
+      "sample": {
+        "uniqueSampleCode": "COB0000000", // identifier of sample
+        "sampleDate": "2020-06-05T00:00:00Z", // date on which the sample is taken
+        "receivedDate": "2020-06-05T00:00:00Z" // date on which the sample is received in the lab
+      },
+      "usedTest": {
+        "testName": "CORONA-NU",
+        "testType": "PCR based SARS-CoV-2 test",
+        "doneByLab": {
+          "id": "", // identifier of test laboratory
+          "name": "CoronaLab.eu"
+        }
+      }
+    }
+  },
+  "proof": {
+    "type": "RsaSignature2018",
+    "created": "2017-06-18T21:19:10Z",
+    "proofPurpose": "assertionMethod",
+    "verificationMethod": "https://example.edu/issuers/keys/1",
+    "jws": "eyJhbGciOiJSUzI1NiIsImI2NCI6ZmFsc2UsImNyaXQiOlsiYjY0Il19..TCYt5XsITJX1CxPCT8yAV-TVkIEq_PbChOMqsLfRoPsnsgw5WEuts01mq-pQy7UJiN5mgRxD-WUcX16dUEMGlv50aqzpqh4Qktb3rk-BuQy72IFLOqV0G_zS245-kronKb78cPN25DGlcTwLtjPAYuNzVBAh4vGHSrQyHUdBBPM"
+  }
+}
+```</t>
+  </si>
+  <si>
+    <t>```
 {
 	"@context": ["https://www.w3.org/2018/credentials/v1", "https://essif.europa.eu/schemas/vc/2020/v1"],
 	"type": ["VerifiableCredential", "VerifiableAttestation", "DiplomaCredential"],
@@ -199,57 +396,11 @@
 		"verificationMethod": "did:ebsi:51rzpDXXCtKExG47boFBahAgd2dtfAZbQxMHM17mYKoq#keys-1",
 		"jws": "eyJiNjQiOmZhbHNlLCJjcml0IjpbImI2NCJdLCJhbGciOiJFUzI1NksifQ..P5vQfWCetyNoCIW6-9cmmdSa1tHPiAaf_bXpQhMrLSUumR4cl5jzfMZsdttlY1HsdcOk1lHJ4nOrItDI0fVrvQ"
 	}
-}</t>
-  </si>
-  <si>
-    <t>https://github.com/danubetech/ebsi4austria-examples
-JSON-LD schema:
-{
-  "@context": {
-    "@version": 1.1,
-    "@protected": true,
-    "id": "@id",
-    "type": "@type",
-    "name": "https://schema.org/name",
-    "description": "https://schema.org/description",
-    "identifier": "http://schema.org/identifier",
-    "image": {"@id": "http://schema.org/image", "@type": "@id"},
-    "essif": "https://essif.europa.eu/schemas/vc/2020/v1#",
-    "xsd": "http://www.w3.org/2001/XMLSchema#",
-    "VerifiableAttestation": "essif:VerifiableAttestation",
-    "DiplomaCredential": "essif:DiplomaCredential",
-    "Student": {
-        "@id": "essif:Student",
-        "@context": {
-            "essif": "https://essif.europa.eu/schemas/vc/2020/v1#",
-            "xsd": "http://www.w3.org/2001/XMLSchema#",
-            "@version": 1.1,
-            "@protected": true,
-            "id": "@id",
-            "type": "@type",
-            "studyProgram": "essif:studyProgram",
-            "immatriculationNumber": "essif:immatriculationNumber",
-            "currentGivenName": "essif:currentGivenName",
-            "currentFamilyName": "essif:currentFamilyName",
-            "learningAchievement": "essif:learningAchievement",
-            "dateOfBirth": { "@id": "essif:dateOfBirth", "@type": "xsd:dateTime" },
-            "dateOfAchievement": { "@id": "essif:dateOfAchievement", "@type": "xsd:dateTime" },
-            "overallEvaluation": "essif:overallEvaluation",
-            "eqfLevel": "essif:eqfLevel",
-            "targetFrameworkName": "essif:targetFrameworkName"
-        }
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>DataKeeper name credential</t>
-  </si>
-  <si>
-    <t>A name as retrieved from a passport</t>
-  </si>
-  <si>
-    <t>example:
+}
+```</t>
+  </si>
+  <si>
+    <t>```
 {
 '@context': [
 'https://www.w3.org/2018/credentials/v1',
@@ -274,66 +425,246 @@
 signatureValue:
 '0a053957ff860a86445a479a75fc1c01bfe405411888fdbad6a3ca374cfd2f5841f394811e7009e3e97e1dc6e7df8dfbfb7571fa461e47a1827741ff5281aff6'
 }
-}</t>
-  </si>
-  <si>
-    <t>VC, datakeeper</t>
-  </si>
-  <si>
-    <t>Marnix.van.den.Bent@rabobank.nl</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>HL Indy Tx Explorer (indyscan.io)</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>INDY ledger</t>
-  </si>
-  <si>
-    <t>ggirc-act.ghg-emissions-report</t>
-  </si>
-  <si>
-    <t>0.2.1</t>
-  </si>
-  <si>
-    <t>{
+}
+```</t>
+  </si>
+  <si>
+    <t>### Attributes:
+- organization_id
+- name_of_farm_natural_person
+- time_of_issuance
+- organization_name_of_issuer
+- district
+- confirmed_by_farmer
+- gps_coordinates_ten
+- name_of_farm
+- gps_coordinates_eight
+- country
+- farm_id
+- address
+- place
+https://indyscan.io/tx/SOVRIN_MAINNET/domain/63347</t>
+  </si>
+  <si>
+    <t>### Attributes:
+- address
+- name_of_farm
+- country
+- place
+- district
+- farm_id
+- time_of_issuance
+- gps_coordinates_ten
+- organization_id
+- organization_name_of_issuer
+- gps_coordinates_eight
+- name_of_farm_natural_person
+https://indyscan.io/tx/SOVRIN_MAINNET/domain/56310</t>
+  </si>
+  <si>
+    <t>### Attributes:
+- effective_date
+- pfcs_emissions
+- primary_activity_code
+- hfcs_emissions
+- issued_date
+- facility_longitude
+- co2_fossil_emissions
+- facility_latitude
+- co2_biomass_emissions
+- registration_id
+- primary_activity_description
+- ch4_emissions
+- n2o_emissions
+- verification_body
+- reporting_year
+- sf6_emissions
+- verification_result
+- facility_name
+https://indyscan.io/tx/SOVRIN_MAINNET/domain/67232</t>
+  </si>
+  <si>
+    <t>###Attributes:
+- testLanguage
+- testResult
+- labCode
+- testType
+- labAddress
+- resultDate
+- labName
+- labPublicPhone
+- takenDate
+- testTechnique
+- testFormat
+- labPublicEmail
+- labPublicWebsite
+- testMethod
+https://indyscan.io/tx/SOVRIN_MAINNET/domain/63152</t>
+  </si>
+  <si>
+    <t>###Attributes:
+- System of Record
+- $Metadata
+- Patient Middle Initial
+- Lot Number
+- Patient Last Name
+- Manufacturer Name
+- Patient Reference Number
+- Administration Date
+- Dose Quantity
+- $Order
+- Vaccine Name
+- Dose Units
+- Lot Expiration
+- Patient First Name
+- $Timestamp
+- Patient Date of Birth
+https://indyscan.io/tx/SOVRIN_MAINNET/domain/62238</t>
+  </si>
+  <si>
+    <t>Your Dutch Citizen service number (BSN), from the Dutch population register, verified face to face
+Credential identifier: pbdf.chipsoft.bsn
+### Attributes
+This credential contains the following attributes:
+- BSN from healthcare: 
+  - Identifier: pbdf.chipsoft.bsn.bsn
+  - Description: Your Dutch Citizen service number (BSN) from healthcare
+- Initials
+  - Identifier: pbdf.chipsoft.bsn.initials
+  - Description: Your initials, abbreviating your first names
+- First names
+  - Identifier: pbdf.chipsoft.bsn.firstnames
+  - Description: Your first names
+- Prefix (optional)
+  - Identifier: pbdf.chipsoft.bsn.prefix
+  - Description: Prefix of your family name
+- Family name
+  - Identifier: pbdf.chipsoft.bsn.familyname
+  - Description: Your family name, as given to you at birth
+- Date of birth
+  - Identifier: pbdf.chipsoft.bsn.dateofbirth
+  - Description: Your date of birth 
+https://privacybydesign.foundation/attribute-index/en/pbdf.chipsoft.bsn.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your home address, from the Dutch population register
+Credential identifier: pbdf.bzkpilot.address
+### Attributes
+- Street
+  - Identifer: pbdf.bzkpilot.address.street
+  - Description: Your street
+ -House number (optional)
+  - Identifer: pbdf.bzkpilot.address.houseNumber
+  - Description: Your house number, with possible extension
+- Postal code
+  - Identifer: pbdf.bzkpilot.address.zipcode
+  - Description: Your postal code
+- City
+  - Identifer: pbdf.bzkpilot.address.city
+  - Description: Your city of residence
+- Municipality
+  - Identifer: pbdf.bzkpilot.address.municipality
+  - Description: Your municipality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your personal data, from the Dutch population register (BRP)
+Credential identifier: pbdf.bzkpilot.personalData
+### Attributes
+- Full name (optional)
+  - Identifier pbdf.bzkpilot.personalData.fullname
+  - Description: Your full family name: your family name or (a combination with) the name of your partner
+- Initials
+  - Identifier pbdf.bzkpilot.personalData.initials
+  - Description: Your initials, abbreviating your first names
+- First names
+  - Identifier pbdf.bzkpilot.personalData.firstnames
+  - Description: Your first names
+- Prefix (optional)
+  - Identifier pbdf.bzkpilot.personalData.prefix
+  - Description: Prefix of your family name
+- Family name
+  - Identifier pbdf.bzkpilot.personalData.familyname
+  - Description: Your family name, as given to you at birth
+- Gender
+  - Identifier pbdf.bzkpilot.personalData.gender
+  - Description: Your gender
+- Date of birth
+  - Identifier pbdf.bzkpilot.personalData.dateofbirth
+  - Description: Your date of birth
+- Over 12
+  - Identifier pbdf.bzkpilot.personalData.over12
+  - Description: Whether you are over 12
+- Over 16
+  - Identifier pbdf.bzkpilot.personalData.over16
+  - Description: Whether you are over 16
+- Over 18
+  - Identifier pbdf.bzkpilot.personalData.over18
+  - Description: Whether you are over 18
+- Over 21
+  - Identifier pbdf.bzkpilot.personalData.over21
+  - Description: Whether you are over 21
+- Over 65
+  - Identifier pbdf.bzkpilot.personalData.over65
+  - Description: Whether you are over 65
+- Dutch nationality (optional)
+  - Identifier pbdf.bzkpilot.personalData.nationality
+  - Description: Whether you have the dutch nationality
+- Country of birth
+  - Identifier pbdf.bzkpilot.personalData.countryofbirth
+  - Description: Your country of birth
+- BSN
+  - Identifier pbdf.bzkpilot.personalData.bsn
+  - Description: Your Dutch Citizen registration number (BSN)
+- Photo
+  - Identifier pbdf.bzkpilot.personalData.photo
+  - Description: Your picture </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An AGB code (in Dutch: Algemeen GegevensBeheer code) is a Dutch national code system which uniquely identifies a care provider. Care providers are registered in a national database with such a code. The database is maintained by Vektis
+Credential identifier: pbdf.nuts.agb
+### Attributes
+- AGB-code
+  - Identifier: pbdf.nuts.agb.agbcode
+  - Description: Uniquely identifying code for individual healthcare professional </t>
+  </si>
+  <si>
+    <t>```
+{
   "txn": {
     "data": {
       "data": {
         "attr_names": [
-          "organization_id",
-          "name_of_farm_natural_person",
-          "time_of_issuance",
-          "organization_name_of_issuer",
-          "district",
-          "confirmed_by_farmer",
-          "gps_coordinates_ten",
-          "name_of_farm",
-          "gps_coordinates_eight",
-          "country",
-          "farm_id",
-          "address",
-          "place"
+          "System of Record",
+          "$Metadata",
+          "Patient Middle Initial",
+          "Lot Number",
+          "Patient Last Name",
+          "Manufacturer Name",
+          "Patient Reference Number",
+          "Administration Date",
+          "Dose Quantity",
+          "$Order",
+          "Vaccine Name",
+          "Dose Units",
+          "Lot Expiration",
+          "Patient First Name",
+          "$Timestamp",
+          "Patient Date of Birth"
         ],
-        "name": "Farm_Schema",
-        "version": "1.2"
+        "name": "COVID-19 Vaccine",
+        "version": "112.11"
       }
     },
     "metadata": {
-      "digest": "d10f941da3f36e56de96c9c6e5cdf53b1f21cef3e9a8a9f7a3827d47d9983d4a",
-      "endorser": "3hzaM4LfEeoZ4wpx324Hjt",
-      "from": "6BrHyg7SoMRmbgQjqJrkcH",
-      "payloadDigest": "b5e11af8c41fb453ab05ca7838ce6b094cf33ab5f00f09dd563a745b9d8d23d6",
-      "reqId": 1626947648269287000,
+      "digest": "91c8a4f0998e07141681284826b75d20d48d97d43e774c7ffa3d4cfeffefad34",
+      "endorser": "NAAVMb535pt7HRNy97zbGP",
+      "from": "8KusBegNmSG2bitSnf14tE",
+      "payloadDigest": "e7242b86ef2e787ec2bf82695ae8b19c7f152708ca3560bfd07fe58e17d9a43a",
+      "reqId": 1625144169009062100,
       "taaAcceptance": {
-        "mechanism": "service_agreement",
+        "mechanism": "on_file",
         "taaDigest": "8cee5d7a573e4893b08ff53a0761a22a1607df3b3fcd7e75b98696c92879641f",
-        "time": 1626912000
+        "time": 1599696000
       }
     },
     "protocolVersion": 2,
@@ -341,48 +672,49 @@
     "typeName": "SCHEMA"
   },
   "txnMetadata": {
-    "seqNo": 63347,
-    "txnId": "6BrHyg7SoMRmbgQjqJrkcH:2:Farm_Schema:1.2",
-    "txnTime": "2021-07-22T09:54:08.000Z"
+    "seqNo": 62237,
+    "txnId": "8KusBegNmSG2bitSnf14tE:2:COVID-19 Vaccine:112.11",
+    "txnTime": "2021-07-01T13:45:42.000Z"
   }
-}</t>
-  </si>
-  <si>
-    <t>Farm_Schema</t>
-  </si>
-  <si>
-    <t>{
+}
+```</t>
+  </si>
+  <si>
+    <t>```
+{
   "txn": {
     "data": {
       "data": {
         "attr_names": [
-          "address",
-          "name_of_farm",
-          "country",
-          "place",
-          "district",
-          "farm_id",
-          "time_of_issuance",
-          "gps_coordinates_ten",
-          "organization_id",
-          "organization_name_of_issuer",
-          "gps_coordinates_eight",
-          "name_of_farm_natural_person"
+          "testLanguage",
+          "testResult",
+          "labCode",
+          "testType",
+          "labAddress",
+          "resultDate",
+          "labName",
+          "labPublicPhone",
+          "takenDate",
+          "testTechnique",
+          "testFormat",
+          "labPublicEmail",
+          "labPublicWebsite",
+          "testMethod"
         ],
-        "name": "Farm_Schema",
-        "version": "1.1"
+        "name": "COVID-19 Test Result",
+        "version": "2.0"
       }
     },
     "metadata": {
-      "digest": "ef930f1b491f896cefcdf3f8a93c3fb246bf73fa9f90c0eb961334b93e316515",
-      "endorser": "3hzaM4LfEeoZ4wpx324Hjt",
-      "from": "39yeYh9n8p7LzWnxbrcqCP",
-      "payloadDigest": "08c02e5096046e8c18d309b625a14e2ae37c9c79b1541bc29f4a44f03550e032",
-      "reqId": 1605688867496636400,
+      "digest": "5a12561025dd9f821b364c10c7c98fc66159b38c747c396867c0678a77499c25",
+      "endorser": "P8u7S3Xz8JD3JvaCGcMyTg",
+      "from": "TTR9ckhm1KNu6g7aBYgxuQ",
+      "payloadDigest": "19f257f8c0f3f073c46feed34916b9c51f474930c1fc4e0837f8d3df980f8947",
+      "reqId": 1626784291061231400,
       "taaAcceptance": {
-        "mechanism": "service_agreement",
+        "mechanism": "at_submission",
         "taaDigest": "8cee5d7a573e4893b08ff53a0761a22a1607df3b3fcd7e75b98696c92879641f",
-        "time": 1605657600
+        "time": 1626739200
       }
     },
     "protocolVersion": 2,
@@ -390,14 +722,16 @@
     "typeName": "SCHEMA"
   },
   "txnMetadata": {
-    "seqNo": 56310,
-    "txnId": "39yeYh9n8p7LzWnxbrcqCP:2:Farm_Schema:1.1",
-    "txnTime": "2020-11-18T08:41:07.000Z"
+    "seqNo": 63152,
+    "txnId": "TTR9ckhm1KNu6g7aBYgxuQ:2:COVID-19 Test Result:2.0",
+    "txnTime": "2021-07-20T12:57:26.000Z"
   }
-}</t>
-  </si>
-  <si>
-    <t>{
+}
+```</t>
+  </si>
+  <si>
+    <t>```
+{
   "txn": {
     "data": {
       "data": {
@@ -446,49 +780,43 @@
     "txnId": "NqFsoG29BHBnczz6t6UBXo:2:ggirc-act.ghg-emissions-report:0.2.1",
     "txnTime": "2021-08-21T18:01:55.000Z"
   }
-}</t>
-  </si>
-  <si>
-    <t>COVID-19 Test Result</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>{
+}
+```</t>
+  </si>
+  <si>
+    <t>```
+{
   "txn": {
     "data": {
       "data": {
         "attr_names": [
-          "testLanguage",
-          "testResult",
-          "labCode",
-          "testType",
-          "labAddress",
-          "resultDate",
-          "labName",
-          "labPublicPhone",
-          "takenDate",
-          "testTechnique",
-          "testFormat",
-          "labPublicEmail",
-          "labPublicWebsite",
-          "testMethod"
+          "address",
+          "name_of_farm",
+          "country",
+          "place",
+          "district",
+          "farm_id",
+          "time_of_issuance",
+          "gps_coordinates_ten",
+          "organization_id",
+          "organization_name_of_issuer",
+          "gps_coordinates_eight",
+          "name_of_farm_natural_person"
         ],
-        "name": "COVID-19 Test Result",
-        "version": "2.0"
+        "name": "Farm_Schema",
+        "version": "1.1"
       }
     },
     "metadata": {
-      "digest": "5a12561025dd9f821b364c10c7c98fc66159b38c747c396867c0678a77499c25",
-      "endorser": "P8u7S3Xz8JD3JvaCGcMyTg",
-      "from": "TTR9ckhm1KNu6g7aBYgxuQ",
-      "payloadDigest": "19f257f8c0f3f073c46feed34916b9c51f474930c1fc4e0837f8d3df980f8947",
-      "reqId": 1626784291061231400,
+      "digest": "ef930f1b491f896cefcdf3f8a93c3fb246bf73fa9f90c0eb961334b93e316515",
+      "endorser": "3hzaM4LfEeoZ4wpx324Hjt",
+      "from": "39yeYh9n8p7LzWnxbrcqCP",
+      "payloadDigest": "08c02e5096046e8c18d309b625a14e2ae37c9c79b1541bc29f4a44f03550e032",
+      "reqId": 1605688867496636400,
       "taaAcceptance": {
-        "mechanism": "at_submission",
+        "mechanism": "service_agreement",
         "taaDigest": "8cee5d7a573e4893b08ff53a0761a22a1607df3b3fcd7e75b98696c92879641f",
-        "time": 1626739200
+        "time": 1605657600
       }
     },
     "protocolVersion": 2,
@@ -496,55 +824,124 @@
     "typeName": "SCHEMA"
   },
   "txnMetadata": {
-    "seqNo": 63152,
-    "txnId": "TTR9ckhm1KNu6g7aBYgxuQ:2:COVID-19 Test Result:2.0",
-    "txnTime": "2021-07-20T12:57:26.000Z"
+    "seqNo": 56310,
+    "txnId": "39yeYh9n8p7LzWnxbrcqCP:2:Farm_Schema:1.1",
+    "txnTime": "2020-11-18T08:41:07.000Z"
   }
-}</t>
-  </si>
-  <si>
-    <t>COVID-19 Vaccine</t>
-  </si>
-  <si>
-    <t>112.11</t>
-  </si>
-  <si>
-    <t>{
+}
+```</t>
+  </si>
+  <si>
+    <t>TxID: Ar1YzNwcM74M2Z4XKUWXMW:2:
+EmploymentSchema:1.0, Seqno: 54019
+- employer
+- employeeID
+- userID
+- email
+- employmentType
+- issuingDate
+- expiryDate
+https://esatus.com/files/whitepapers/esatus_SSI_Roll-out.pdf</t>
+  </si>
+  <si>
+    <t>TxID: Ar1YzNwcM74M2Z4XKUWXMW:2:
+DepartmentMemberSchema:1.0, Seqno: 54020
+- position
+- location
+- departmentID
+- department
+- issuingDate
+- expiryDate
+https://esatus.com/files/whitepapers/esatus_SSI_Roll-out.pdf</t>
+  </si>
+  <si>
+    <t>TxID: Ar1YzNwcM74M2Z4XKUWXMW:2:
+ProjectMemberSchema:1.0, Seqno: 54021
+- role
+- projectID
+- project
+- issuingDate
+- expiryDate
+https://esatus.com/files/whitepapers/esatus_SSI_Roll-out.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/danubetech/ebsi4austria-examples
+JSON-LD schema:
+```
+{
+  "@context": {
+    "@version": 1.1,
+    "@protected": true,
+    "id": "@id",
+    "type": "@type",
+    "name": "https://schema.org/name",
+    "description": "https://schema.org/description",
+    "identifier": "http://schema.org/identifier",
+    "image": {"@id": "http://schema.org/image", "@type": "@id"},
+    "essif": "https://essif.europa.eu/schemas/vc/2020/v1#",
+    "xsd": "http://www.w3.org/2001/XMLSchema#",
+    "VerifiableAttestation": "essif:VerifiableAttestation",
+    "DiplomaCredential": "essif:DiplomaCredential",
+    "Student": {
+        "@id": "essif:Student",
+        "@context": {
+            "essif": "https://essif.europa.eu/schemas/vc/2020/v1#",
+            "xsd": "http://www.w3.org/2001/XMLSchema#",
+            "@version": 1.1,
+            "@protected": true,
+            "id": "@id",
+            "type": "@type",
+            "studyProgram": "essif:studyProgram",
+            "immatriculationNumber": "essif:immatriculationNumber",
+            "currentGivenName": "essif:currentGivenName",
+            "currentFamilyName": "essif:currentFamilyName",
+            "learningAchievement": "essif:learningAchievement",
+            "dateOfBirth": { "@id": "essif:dateOfBirth", "@type": "xsd:dateTime" },
+            "dateOfAchievement": { "@id": "essif:dateOfAchievement", "@type": "xsd:dateTime" },
+            "overallEvaluation": "essif:overallEvaluation",
+            "eqfLevel": "essif:eqfLevel",
+            "targetFrameworkName": "essif:targetFrameworkName"
+        }
+    }
+  }
+}
+```</t>
+  </si>
+  <si>
+    <t>```
+{
   "txn": {
     "data": {
       "data": {
         "attr_names": [
-          "System of Record",
-          "$Metadata",
-          "Patient Middle Initial",
-          "Lot Number",
-          "Patient Last Name",
-          "Manufacturer Name",
-          "Patient Reference Number",
-          "Administration Date",
-          "Dose Quantity",
-          "$Order",
-          "Vaccine Name",
-          "Dose Units",
-          "Lot Expiration",
-          "Patient First Name",
-          "$Timestamp",
-          "Patient Date of Birth"
+          "organization_id",
+          "name_of_farm_natural_person",
+          "time_of_issuance",
+          "organization_name_of_issuer",
+          "district",
+          "confirmed_by_farmer",
+          "gps_coordinates_ten",
+          "name_of_farm",
+          "gps_coordinates_eight",
+          "country",
+          "farm_id",
+          "address",
+          "place"
         ],
-        "name": "COVID-19 Vaccine",
-        "version": "112.11"
+        "name": "Farm_Schema",
+        "version": "1.2"
       }
     },
     "metadata": {
-      "digest": "91c8a4f0998e07141681284826b75d20d48d97d43e774c7ffa3d4cfeffefad34",
-      "endorser": "NAAVMb535pt7HRNy97zbGP",
-      "from": "8KusBegNmSG2bitSnf14tE",
-      "payloadDigest": "e7242b86ef2e787ec2bf82695ae8b19c7f152708ca3560bfd07fe58e17d9a43a",
-      "reqId": 1625144169009062100,
+      "digest": "d10f941da3f36e56de96c9c6e5cdf53b1f21cef3e9a8a9f7a3827d47d9983d4a",
+      "endorser": "3hzaM4LfEeoZ4wpx324Hjt",
+      "from": "6BrHyg7SoMRmbgQjqJrkcH",
+      "payloadDigest": "b5e11af8c41fb453ab05ca7838ce6b094cf33ab5f00f09dd563a745b9d8d23d6",
+      "reqId": 1626947648269287000,
       "taaAcceptance": {
-        "mechanism": "on_file",
+        "mechanism": "service_agreement",
         "taaDigest": "8cee5d7a573e4893b08ff53a0761a22a1607df3b3fcd7e75b98696c92879641f",
-        "time": 1599696000
+        "time": 1626912000
       }
     },
     "protocolVersion": 2,
@@ -552,109 +949,12 @@
     "typeName": "SCHEMA"
   },
   "txnMetadata": {
-    "seqNo": 62237,
-    "txnId": "8KusBegNmSG2bitSnf14tE:2:COVID-19 Vaccine:112.11",
-    "txnTime": "2021-07-01T13:45:42.000Z"
+    "seqNo": 63347,
+    "txnId": "6BrHyg7SoMRmbgQjqJrkcH:2:Farm_Schema:1.2",
+    "txnTime": "2021-07-22T09:54:08.000Z"
   }
-}</t>
-  </si>
-  <si>
-    <t>https://gitlab.com/RoosBakker/coti</t>
-  </si>
-  <si>
-    <t>Stores the result of a LAMP quicktest for COVID 19
-example:
-{
-  "@context": [
-    "https://www.w3.org/2018/credentials/v1",
-    "https://www.tno.nl/health/ontology/coti" // TODO: location of schema
-  ],
-  "id": "https://ns.unlock.nl/credentials/example/2",
-  "type": ["VerifiableCredential", "COVID19LAMPTestResultCredential"],
-  "issuer": "did:example:c276e12ec21ebfeb1f712ebc6f1",
-  "issuanceDate": "2020-12-10T19:73:24Z",
-  "credentialSubject": {
-    "id": "did:example:ebfeb1f712ebc6f1c276e12ec21", // did of unlock wallet
-    "passportPhotograph": "iVBORw0KGgoAAAANSUhEUgAAAuAAAACFCAIAAACVGtqeAAAAA3", // string of the image
-    "testResult": {
-      "date": "2020-12-10T00:00:00Z", // datetime on which the test result is specified
-      "result": false,
-      "usedTest": {
-        "testName": "TNOLAMP",
-        "testType": "LAMP based SARS-CoV-2 test",
-        "doneByLab": {
-          "id": "https://tno.nl", // identifier of test laboratory
-          "name": "TNO"
-        }
-      }
-    }
-  },
-  "proof": {
-    "type": "RsaSignature2018",
-    "created": "2017-06-18T21:19:10Z",
-    "proofPurpose": "assertionMethod",
-    "verificationMethod": "https://example.edu/issuers/keys/1",
-    "jws": "eyJhbGciOiJSUzI1NiIsImI2NCI6ZmFsc2UsImNyaXQiOlsiYjY0Il19..TCYt5XsITJX1CxPCT8yAV-TVkIEq_PbChOMqsLfRoPsnsgw5WEuts01mq-pQy7UJiN5mgRxD-WUcX16dUEMGlv50aqzpqh4Qktb3rk-BuQy72IFLOqV0G_zS245-kronKb78cPN25DGlcTwLtjPAYuNzVBAh4vGHSrQyHUdBBPM"
-  }
-}</t>
-  </si>
-  <si>
-    <t>Stores the result of an antigetn quicktest for COVID 19
-example:
-{
-  "@context": [
-    "https://www.w3.org/2018/credentials/v1",
-    "https://www.tno.nl/health/ontology/coti" // TODO: location of schema
-  ],
-  "id": "https://ns.unlock.nl/credentials/example/2",
-  "type": ["VerifiableCredential", "COVID19AntigenTestResultCredential"],
-  "issuer": "did:example:c276e12ec21ebfeb1f712ebc6f1",
-  "issuanceDate": "2020-12-10T19:73:24Z",
-  "credentialSubject": {
-    "id": "did:example:ebfeb1f712ebc6f1c276e12ec21", // did of unlock wallet
-    "passportPhotograph": "iVBORw0KGgoAAAANSUhEUgAAAuAAAACFCAIAAACVGtqeAAAAA3", // string of the image
-    "testResult": {
-      "date": "2020-12-10T00:00:00Z", // datetime on which the test result is specified
-      "result": false,
-      "usedTest": {
-        "testName": "Abbott",
-        "testType": "Antigen based SARS-CoV-2 test",
-        "doneByLab": {
-          "id": "https://ems.eu", // identifier of test laboratory
-          "name": "EMS"
-        }
-      }
-    }
-  },
-  "proof": {
-    "type": "RsaSignature2018",
-    "created": "2017-06-18T21:19:10Z",
-    "proofPurpose": "assertionMethod",
-    "verificationMethod": "https://example.edu/issuers/keys/1",
-    "jws": "eyJhbGciOiJSUzI1NiIsImI2NCI6ZmFsc2UsImNyaXQiOlsiYjY0Il19..TCYt5XsITJX1CxPCT8yAV-TVkIEq_PbChOMqsLfRoPsnsgw5WEuts01mq-pQy7UJiN5mgRxD-WUcX16dUEMGlv50aqzpqh4Qktb3rk-BuQy72IFLOqV0G_zS245-kronKb78cPN25DGlcTwLtjPAYuNzVBAh4vGHSrQyHUdBBPM"
-  }
-}</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>documentation</t>
-  </si>
-  <si>
-    <t>supportedProts</t>
-  </si>
-  <si>
-    <t>maturity</t>
-  </si>
-  <si>
-    <t>contact</t>
+}
+```</t>
   </si>
 </sst>
 </file>
@@ -693,9 +993,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -780,11 +1078,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -805,7 +1102,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -818,12 +1114,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="159">
@@ -3355,7 +3648,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF05A35E-27A3-42DB-92DF-32CE8E881D77}" name="Table2" displayName="Table2" ref="B1:CB7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="158">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF05A35E-27A3-42DB-92DF-32CE8E881D77}" name="Table2" displayName="Table2" ref="B1:CB8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="158">
   <tableColumns count="79">
     <tableColumn id="1" xr3:uid="{99DD80C4-89D5-4772-BFB9-B45AA3C6865B}" name="Column1" headerRowDxfId="157" dataDxfId="156"/>
     <tableColumn id="2" xr3:uid="{91DEF50E-BA31-4F6C-B2B7-FBFED5D1D8E6}" name="Column2" headerRowDxfId="155" dataDxfId="154"/>
@@ -3738,25 +4031,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99EF979-9ACD-42FD-AF69-EB30268A5960}">
-  <dimension ref="A1:CB7"/>
+  <dimension ref="A1:CB8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.6640625" style="3" customWidth="1"/>
-    <col min="4" max="16" width="52.6640625" customWidth="1"/>
-    <col min="17" max="17" width="40.6640625" customWidth="1"/>
-    <col min="18" max="80" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" style="3" customWidth="1"/>
+    <col min="4" max="29" width="55.6640625" customWidth="1"/>
+    <col min="30" max="80" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="6" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -3774,424 +4066,446 @@
         <v>13</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:80" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:80" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>57</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="15" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="14"/>
+      <c r="AQ2" s="14"/>
+      <c r="AR2" s="14"/>
+      <c r="AS2" s="14"/>
+      <c r="AT2" s="14"/>
+      <c r="AU2" s="14"/>
+      <c r="AV2" s="14"/>
+      <c r="AW2" s="14"/>
+      <c r="AX2" s="14"/>
+      <c r="AY2" s="14"/>
+      <c r="AZ2" s="14"/>
+      <c r="BA2" s="14"/>
+      <c r="BB2" s="14"/>
+      <c r="BC2" s="14"/>
+      <c r="BD2" s="14"/>
+      <c r="BE2" s="14"/>
+      <c r="BF2" s="14"/>
+      <c r="BG2" s="14"/>
+      <c r="BH2" s="14"/>
+      <c r="BI2" s="14"/>
+      <c r="BJ2" s="14"/>
+      <c r="BK2" s="14"/>
+      <c r="BL2" s="14"/>
+      <c r="BM2" s="14"/>
+      <c r="BN2" s="14"/>
+      <c r="BO2" s="14"/>
+      <c r="BP2" s="14"/>
+      <c r="BQ2" s="14"/>
+      <c r="BR2" s="14"/>
+      <c r="BS2" s="14"/>
+      <c r="BT2" s="14"/>
+      <c r="BU2" s="14"/>
+      <c r="BV2" s="14"/>
+      <c r="BW2" s="14"/>
+      <c r="BX2" s="14"/>
+      <c r="BY2" s="14"/>
+      <c r="BZ2" s="14"/>
+      <c r="CA2" s="14"/>
+      <c r="CB2" s="14"/>
+    </row>
+    <row r="3" spans="1:80" s="17" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:80" s="17" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:80" s="17" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="15"/>
-      <c r="AS2" s="15"/>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15"/>
-      <c r="AV2" s="15"/>
-      <c r="AW2" s="15"/>
-      <c r="AX2" s="15"/>
-      <c r="AY2" s="15"/>
-      <c r="AZ2" s="15"/>
-      <c r="BA2" s="15"/>
-      <c r="BB2" s="15"/>
-      <c r="BC2" s="15"/>
-      <c r="BD2" s="15"/>
-      <c r="BE2" s="15"/>
-      <c r="BF2" s="15"/>
-      <c r="BG2" s="15"/>
-      <c r="BH2" s="15"/>
-      <c r="BI2" s="15"/>
-      <c r="BJ2" s="15"/>
-      <c r="BK2" s="15"/>
-      <c r="BL2" s="15"/>
-      <c r="BM2" s="15"/>
-      <c r="BN2" s="15"/>
-      <c r="BO2" s="15"/>
-      <c r="BP2" s="15"/>
-      <c r="BQ2" s="15"/>
-      <c r="BR2" s="15"/>
-      <c r="BS2" s="15"/>
-      <c r="BT2" s="15"/>
-      <c r="BU2" s="15"/>
-      <c r="BV2" s="15"/>
-      <c r="BW2" s="15"/>
-      <c r="BX2" s="15"/>
-      <c r="BY2" s="15"/>
-      <c r="BZ2" s="15"/>
-      <c r="CA2" s="15"/>
-      <c r="CB2" s="15"/>
-    </row>
-    <row r="3" spans="1:80" s="18" customFormat="1" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17" t="s">
+      <c r="D5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:80" s="18" customFormat="1" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:80" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>40</v>
+      <c r="Q5" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:80" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:80" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>19</v>
+      <c r="F7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:80" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="10" t="s">
+    <row r="8" spans="1:80" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="12" t="s">
+      <c r="F8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1" display="https://gitlab.com/RoosBakker" xr:uid="{3ABEAD96-E2F9-44E0-9399-4564A6114274}"/>
-    <hyperlink ref="D7" r:id="rId2" display="https://gitlab.com/RoosBakker" xr:uid="{B81EAF04-0952-40E9-9222-F6F65E0AA482}"/>
-    <hyperlink ref="E7" r:id="rId3" display="https://gitlab.com/RoosBakker" xr:uid="{79A629DB-78F4-40B5-ADBA-BEDD9226D5C0}"/>
-    <hyperlink ref="I7" r:id="rId4" display="mailto:markus@danubetech.com" xr:uid="{7A223551-4390-41C5-8839-79A188A61A5C}"/>
-    <hyperlink ref="J7" r:id="rId5" xr:uid="{37739FC1-46DE-408D-8BCD-9D5C87EB04A5}"/>
-    <hyperlink ref="K4" r:id="rId6" display="https://indyscan.io/tx/SOVRIN_MAINNET/domain/63347" xr:uid="{AC569B34-012F-4182-A8C9-1233089A3737}"/>
-    <hyperlink ref="L4" r:id="rId7" display="https://indyscan.io/tx/SOVRIN_MAINNET/domain/56310" xr:uid="{586A2450-7F0C-41EC-9564-E6005A790BF0}"/>
-    <hyperlink ref="M4" r:id="rId8" display="https://indyscan.io/tx/SOVRIN_MAINNET/domain/67232" xr:uid="{DD6CFA9E-2F16-46D3-8C78-23590DD51AFD}"/>
-    <hyperlink ref="N4" r:id="rId9" display="https://indyscan.io/tx/SOVRIN_MAINNET/domain/63152" xr:uid="{100B6046-8D74-46C9-8856-B99379962DCB}"/>
-    <hyperlink ref="O4" r:id="rId10" display="https://indyscan.io/tx/SOVRIN_MAINNET/domain/62237" xr:uid="{5CD554EA-BD2A-423F-8EF9-10476EC9937E}"/>
-    <hyperlink ref="C4" r:id="rId11" xr:uid="{13FAC05F-48ED-48BC-9963-1E57DBCC15A6}"/>
-    <hyperlink ref="D4" r:id="rId12" xr:uid="{CF058C10-B7C8-449A-84FA-A120116C82D8}"/>
-    <hyperlink ref="E4" r:id="rId13" xr:uid="{AFC10C44-BF3B-4B0B-82F0-D9A6EE4AB99A}"/>
-  </hyperlinks>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Team Document" ma:contentTypeID="0x010100A35317DCC28344A7B82488658A034A5C010078A2599E1C404E4596119BE342CA2038" ma:contentTypeVersion="13" ma:contentTypeDescription=" " ma:contentTypeScope="" ma:versionID="a601b4647638f03f4a8aea2a02022eeb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="310caa71-58aa-4a5b-bfda-3b9f0b511c38" xmlns:ns3="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7" xmlns:ns5="00b49fb4-9c02-4a1e-9bff-9ec2284fe8b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="81feba35e50249d0e856ffbbbf634929" ns2:_="" ns3:_="" ns5:_="">
     <xsd:import namespace="310caa71-58aa-4a5b-bfda-3b9f0b511c38"/>
@@ -4518,7 +4832,66 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lca20d149a844688b6abf34073d5c21d xmlns="310caa71-58aa-4a5b-bfda-3b9f0b511c38">
@@ -4569,24 +4942,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6712A797-5D2D-4C14-B8A8-D1B2C820D388}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F20F2220-D5AC-4306-8D59-8ABD4A7D0933}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4606,7 +4962,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6712A797-5D2D-4C14-B8A8-D1B2C820D388}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AFB4984-1458-4F8C-9561-0E4D3B3ACA8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5C59D7-1C63-43F3-A9DF-6C752E077EFB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4616,12 +4988,4 @@
     <ds:schemaRef ds:uri="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AFB4984-1458-4F8C-9561-0E4D3B3ACA8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>